<commit_message>
v0.3 modelado de DB proyectos, creador, tipo en Dublin Core
</commit_message>
<xml_diff>
--- a/data/Listado de proyectos digitales BRC.xlsx
+++ b/data/Listado de proyectos digitales BRC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Proyectos digitales" sheetId="1" state="visible" r:id="rId2"/>
@@ -1057,7 +1057,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1090,6 +1090,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1134,7 +1140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1159,6 +1165,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,7 +1192,7 @@
   </sheetPr>
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4325,19 +4339,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B95"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="6" t="s">
         <v>338</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -4345,41 +4360,65 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="n">
+        <v>4</v>
+      </c>
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="n">
+        <v>5</v>
+      </c>
       <c r="B6" s="3" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="n">
+        <v>6</v>
+      </c>
       <c r="B7" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="n">
+        <v>7</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="n">
+        <v>8</v>
+      </c>
       <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
@@ -4395,6 +4434,9 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3"/>

</xml_diff>